<commit_message>
All bat files added
</commit_message>
<xml_diff>
--- a/excel/Template.xlsx
+++ b/excel/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daary\PycharmProjects\WebscrapingSuite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4999BC70-86B6-4168-889C-149C638DFC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79F202B-13BE-49BB-8844-43513AEF3A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AF14A077-A23C-4913-8C40-7CFF0597FBC4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AF14A077-A23C-4913-8C40-7CFF0597FBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="10" r:id="rId1"/>
@@ -1671,95 +1671,95 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="34" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2078,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F317D1DB-5C3E-4320-8ED1-BC4F63A69614}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2117,7 +2117,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2142,7 +2142,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="109" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2151,42 +2151,42 @@
         <v>143</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="80"/>
+      <c r="C8" s="109"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>144</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="80"/>
+      <c r="C9" s="109"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>145</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="80"/>
+      <c r="C10" s="109"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>146</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="80"/>
+      <c r="C11" s="109"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>147</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="80"/>
+      <c r="C12" s="109"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>148</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="80"/>
+      <c r="C13" s="109"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
@@ -2194,93 +2194,93 @@
       </c>
       <c r="B14" s="3" t="b">
         <f>B4</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="80"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="109"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>150</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="80"/>
+      <c r="C15" s="109"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>151</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="80"/>
+      <c r="C16" s="109"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>152</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="80"/>
+      <c r="C17" s="109"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>153</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="80"/>
+      <c r="C18" s="109"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>154</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="80"/>
+      <c r="C19" s="109"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="80"/>
+      <c r="C20" s="109"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>155</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="80"/>
+      <c r="C21" s="109"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>156</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="80"/>
+      <c r="C22" s="109"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>157</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="80"/>
+      <c r="C23" s="109"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>158</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="80"/>
+      <c r="C24" s="109"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>159</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="80"/>
+      <c r="C25" s="109"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
         <v>160</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="80"/>
+      <c r="C26" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2304,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84FBC5B-DDF7-4192-94E1-360D45BEDC8B}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
@@ -2370,1050 +2370,1050 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="84" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="87" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="88" t="s">
+      <c r="K2" s="87" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="86"/>
+      <c r="L2" s="85"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="92" t="s">
+      <c r="B3" s="89"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="93" t="s">
+      <c r="E3" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="96" t="s">
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="L3" s="95"/>
+      <c r="L3" s="94"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="97" t="s">
         <v>225</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="92" t="s">
+      <c r="B4" s="89"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="96" t="s">
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="97" t="s">
+      <c r="K4" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="95"/>
+      <c r="L4" s="94"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="99"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="92" t="s">
+      <c r="A5" s="98"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="96" t="s">
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="93"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="95"/>
+      <c r="L5" s="94"/>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="99"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="92" t="s">
+      <c r="A6" s="98"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="97" t="s">
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="L6" s="95"/>
+      <c r="L6" s="94"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="99"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92" t="s">
+      <c r="A7" s="98"/>
+      <c r="B7" s="89"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="97" t="s">
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="L7" s="95"/>
+      <c r="L7" s="94"/>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="99"/>
-      <c r="B8" s="90"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="92" t="s">
+      <c r="A8" s="98"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="93" t="s">
+      <c r="E8" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="95"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="97" t="s">
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="93"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="96" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="95"/>
+      <c r="L8" s="94"/>
     </row>
     <row r="9" spans="1:14" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="99"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="92" t="s">
+      <c r="A9" s="98"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="93" t="s">
+      <c r="E9" s="92" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="91"/>
-      <c r="K9" s="97" t="s">
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="L9" s="95"/>
+      <c r="L9" s="94"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="99"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="92" t="s">
+      <c r="A10" s="98"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="94"/>
-      <c r="F10" s="93" t="s">
+      <c r="E10" s="93"/>
+      <c r="F10" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="91"/>
-      <c r="K10" s="97" t="s">
+      <c r="G10" s="93"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="96" t="s">
         <v>94</v>
       </c>
-      <c r="L10" s="95"/>
+      <c r="L10" s="94"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="99"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="92" t="s">
+      <c r="A11" s="98"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="91" t="s">
         <v>176</v>
       </c>
-      <c r="E11" s="94"/>
-      <c r="F11" s="93" t="s">
+      <c r="E11" s="93"/>
+      <c r="F11" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="97" t="s">
+      <c r="G11" s="93"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="96" t="s">
         <v>75</v>
       </c>
-      <c r="L11" s="95"/>
+      <c r="L11" s="94"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="99"/>
-      <c r="B12" s="90"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="92" t="s">
+      <c r="A12" s="98"/>
+      <c r="B12" s="89"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="94"/>
-      <c r="F12" s="93" t="s">
+      <c r="E12" s="93"/>
+      <c r="F12" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G12" s="94"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="91"/>
-      <c r="K12" s="97" t="s">
+      <c r="G12" s="93"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="94"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="L12" s="101" t="s">
+      <c r="L12" s="100" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="99"/>
-      <c r="B13" s="90"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="92" t="s">
+      <c r="A13" s="98"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="94"/>
-      <c r="F13" s="93" t="s">
+      <c r="E13" s="93"/>
+      <c r="F13" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="97" t="s">
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="94"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="L13" s="101" t="s">
+      <c r="L13" s="100" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="99"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="92" t="s">
+      <c r="A14" s="98"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="94"/>
-      <c r="F14" s="93" t="s">
+      <c r="E14" s="93"/>
+      <c r="F14" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="95"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="97" t="s">
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="96" t="s">
         <v>98</v>
       </c>
-      <c r="L14" s="101" t="s">
+      <c r="L14" s="100" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="99"/>
-      <c r="B15" s="90"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="92" t="s">
+      <c r="A15" s="98"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="94"/>
-      <c r="F15" s="93" t="s">
+      <c r="E15" s="93"/>
+      <c r="F15" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="95"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="97" t="s">
+      <c r="G15" s="93"/>
+      <c r="H15" s="93"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="101" t="s">
+      <c r="L15" s="100" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="99"/>
-      <c r="B16" s="90"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="92" t="s">
+      <c r="A16" s="98"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="94"/>
-      <c r="F16" s="93" t="s">
+      <c r="E16" s="93"/>
+      <c r="F16" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G16" s="94"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="97" t="s">
+      <c r="G16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="94"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="96" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="101" t="s">
+      <c r="L16" s="100" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="99"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="92" t="s">
+      <c r="A17" s="98"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="94"/>
-      <c r="F17" s="93" t="s">
+      <c r="E17" s="93"/>
+      <c r="F17" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="97" t="s">
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="L17" s="101" t="s">
+      <c r="L17" s="100" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="99"/>
-      <c r="B18" s="90"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="92" t="s">
+      <c r="A18" s="98"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="92" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G18" s="94"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="91"/>
-      <c r="K18" s="97" t="s">
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="L18" s="101" t="s">
+      <c r="L18" s="100" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="99"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="92" t="s">
+      <c r="A19" s="98"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="94"/>
-      <c r="F19" s="93" t="s">
+      <c r="E19" s="93"/>
+      <c r="F19" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G19" s="94"/>
-      <c r="H19" s="94"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="91"/>
-      <c r="K19" s="97" t="s">
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="L19" s="101" t="s">
+      <c r="L19" s="100" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="99"/>
-      <c r="B20" s="90"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="92" t="s">
+      <c r="A20" s="98"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="94"/>
-      <c r="F20" s="93" t="s">
+      <c r="E20" s="93"/>
+      <c r="F20" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G20" s="94"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="97" t="s">
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="94"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="L20" s="101" t="s">
+      <c r="L20" s="100" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="99"/>
-      <c r="B21" s="90"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="92" t="s">
+      <c r="A21" s="98"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="93" t="s">
+      <c r="E21" s="93"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="I21" s="95"/>
-      <c r="J21" s="91"/>
-      <c r="K21" s="97" t="s">
+      <c r="I21" s="94"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="96" t="s">
         <v>105</v>
       </c>
-      <c r="L21" s="101" t="s">
+      <c r="L21" s="100" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="99"/>
-      <c r="B22" s="90"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="92" t="s">
+      <c r="A22" s="98"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="94"/>
-      <c r="I22" s="95"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="97" t="s">
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="96" t="s">
         <v>106</v>
       </c>
-      <c r="L22" s="101" t="s">
+      <c r="L22" s="100" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="99"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="92" t="s">
+      <c r="A23" s="98"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="97" t="s">
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="93"/>
+      <c r="H23" s="93"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="L23" s="101" t="s">
+      <c r="L23" s="100" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="99"/>
-      <c r="B24" s="90"/>
-      <c r="C24" s="91"/>
-      <c r="D24" s="92" t="s">
+      <c r="A24" s="98"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="91" t="s">
         <v>201</v>
       </c>
-      <c r="E24" s="94"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="94"/>
-      <c r="I24" s="95"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="97" t="s">
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="93"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="L24" s="101" t="s">
+      <c r="L24" s="100" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="99"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="92" t="s">
+      <c r="A25" s="98"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="91" t="s">
         <v>204</v>
       </c>
-      <c r="E25" s="94"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="94"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="95"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="97" t="s">
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="94"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="L25" s="101" t="s">
+      <c r="L25" s="100" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="99"/>
-      <c r="B26" s="90"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="92" t="s">
+      <c r="A26" s="98"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="94"/>
-      <c r="F26" s="94"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="93" t="s">
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="I26" s="95"/>
-      <c r="J26" s="91"/>
-      <c r="K26" s="97" t="s">
+      <c r="I26" s="94"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="L26" s="101" t="s">
+      <c r="L26" s="100" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="99"/>
-      <c r="B27" s="90"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="92" t="s">
+      <c r="A27" s="98"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="94"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="94"/>
-      <c r="I27" s="101" t="s">
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="J27" s="91"/>
-      <c r="K27" s="97" t="s">
+      <c r="J27" s="90"/>
+      <c r="K27" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="L27" s="95"/>
+      <c r="L27" s="94"/>
     </row>
     <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="99"/>
-      <c r="B28" s="90"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="92" t="s">
+      <c r="A28" s="98"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="101" t="s">
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="93"/>
+      <c r="H28" s="93"/>
+      <c r="I28" s="100" t="s">
         <v>185</v>
       </c>
-      <c r="J28" s="91"/>
-      <c r="K28" s="97" t="s">
+      <c r="J28" s="90"/>
+      <c r="K28" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="L28" s="95"/>
+      <c r="L28" s="94"/>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="99"/>
-      <c r="B29" s="90"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="92" t="s">
+      <c r="A29" s="98"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="94"/>
-      <c r="F29" s="93" t="s">
+      <c r="E29" s="93"/>
+      <c r="F29" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="G29" s="94"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="95"/>
-      <c r="J29" s="91"/>
-      <c r="K29" s="97" t="s">
+      <c r="G29" s="93"/>
+      <c r="H29" s="93"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="L29" s="95"/>
+      <c r="L29" s="94"/>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="99"/>
-      <c r="B30" s="90"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="92" t="s">
+      <c r="A30" s="98"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="91" t="s">
         <v>200</v>
       </c>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="95"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="97" t="s">
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="93"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="L30" s="95"/>
+      <c r="L30" s="94"/>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="99"/>
-      <c r="B31" s="90"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="92" t="s">
+      <c r="A31" s="98"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="91" t="s">
         <v>202</v>
       </c>
-      <c r="E31" s="94"/>
-      <c r="F31" s="94"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="94"/>
-      <c r="I31" s="95"/>
-      <c r="J31" s="91"/>
-      <c r="K31" s="97" t="s">
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="90"/>
+      <c r="K31" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="L31" s="95"/>
+      <c r="L31" s="94"/>
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="99"/>
-      <c r="B32" s="90"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="102" t="s">
+      <c r="A32" s="98"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="94"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="95"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="97" t="s">
+      <c r="E32" s="93"/>
+      <c r="F32" s="93"/>
+      <c r="G32" s="93"/>
+      <c r="H32" s="93"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="L32" s="95"/>
+      <c r="L32" s="94"/>
     </row>
     <row r="33" spans="1:12" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="99"/>
-      <c r="B33" s="90"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="102" t="s">
+      <c r="A33" s="98"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="93" t="s">
+      <c r="E33" s="92" t="s">
         <v>177</v>
       </c>
-      <c r="F33" s="94"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="101" t="s">
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="100" t="s">
         <v>175</v>
       </c>
-      <c r="J33" s="91"/>
-      <c r="K33" s="97" t="s">
+      <c r="J33" s="90"/>
+      <c r="K33" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="L33" s="95"/>
+      <c r="L33" s="94"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="99"/>
-      <c r="B34" s="90"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="92" t="s">
+      <c r="A34" s="98"/>
+      <c r="B34" s="89"/>
+      <c r="C34" s="90"/>
+      <c r="D34" s="91" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="94"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="97" t="s">
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="94"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="96" t="s">
         <v>118</v>
       </c>
-      <c r="L34" s="95"/>
+      <c r="L34" s="94"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="99"/>
-      <c r="B35" s="90"/>
-      <c r="C35" s="91"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="94"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="94"/>
-      <c r="I35" s="95"/>
-      <c r="J35" s="91"/>
-      <c r="K35" s="97" t="s">
+      <c r="A35" s="98"/>
+      <c r="B35" s="89"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="93"/>
+      <c r="H35" s="93"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="96" t="s">
         <v>119</v>
       </c>
-      <c r="L35" s="95"/>
+      <c r="L35" s="94"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="99"/>
-      <c r="B36" s="90"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="105"/>
-      <c r="F36" s="105"/>
-      <c r="G36" s="105"/>
-      <c r="H36" s="105"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="91"/>
-      <c r="K36" s="97" t="s">
+      <c r="A36" s="98"/>
+      <c r="B36" s="89"/>
+      <c r="C36" s="90"/>
+      <c r="D36" s="103"/>
+      <c r="E36" s="104"/>
+      <c r="F36" s="104"/>
+      <c r="G36" s="104"/>
+      <c r="H36" s="104"/>
+      <c r="I36" s="105"/>
+      <c r="J36" s="90"/>
+      <c r="K36" s="96" t="s">
         <v>120</v>
       </c>
-      <c r="L36" s="95"/>
+      <c r="L36" s="94"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="99"/>
-      <c r="B37" s="90"/>
-      <c r="C37" s="90"/>
-      <c r="D37" s="90"/>
-      <c r="E37" s="90"/>
-      <c r="F37" s="90"/>
-      <c r="G37" s="90"/>
-      <c r="H37" s="90"/>
-      <c r="I37" s="91"/>
-      <c r="J37" s="91"/>
-      <c r="K37" s="97" t="s">
+      <c r="A37" s="98"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="89"/>
+      <c r="D37" s="89"/>
+      <c r="E37" s="89"/>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89"/>
+      <c r="I37" s="90"/>
+      <c r="J37" s="90"/>
+      <c r="K37" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="L37" s="95"/>
+      <c r="L37" s="94"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="99"/>
-      <c r="B38" s="90"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="90"/>
-      <c r="G38" s="90"/>
-      <c r="H38" s="90"/>
-      <c r="I38" s="91"/>
-      <c r="J38" s="91"/>
-      <c r="K38" s="97" t="s">
+      <c r="A38" s="98"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="90"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="L38" s="101" t="s">
+      <c r="L38" s="100" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="99"/>
-      <c r="B39" s="90"/>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="90"/>
-      <c r="G39" s="90"/>
-      <c r="H39" s="90"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="97" t="s">
+      <c r="A39" s="98"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="89"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="L39" s="101" t="s">
+      <c r="L39" s="100" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="99"/>
-      <c r="B40" s="90"/>
-      <c r="C40" s="90"/>
-      <c r="D40" s="90"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="90"/>
-      <c r="G40" s="90"/>
-      <c r="H40" s="90"/>
-      <c r="I40" s="91"/>
-      <c r="J40" s="91"/>
-      <c r="K40" s="97" t="s">
+      <c r="A40" s="98"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="89"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="L40" s="101" t="s">
+      <c r="L40" s="100" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="99"/>
-      <c r="B41" s="90"/>
-      <c r="C41" s="90"/>
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="90"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="91"/>
-      <c r="J41" s="91"/>
-      <c r="K41" s="97" t="s">
+      <c r="A41" s="98"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="90"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="L41" s="101" t="s">
+      <c r="L41" s="100" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="99"/>
-      <c r="B42" s="90"/>
-      <c r="C42" s="90"/>
-      <c r="D42" s="90"/>
-      <c r="E42" s="90"/>
-      <c r="F42" s="90"/>
-      <c r="G42" s="90"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="91"/>
-      <c r="J42" s="91"/>
-      <c r="K42" s="97" t="s">
+      <c r="A42" s="98"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="89"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="89"/>
+      <c r="H42" s="89"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="L42" s="101" t="s">
+      <c r="L42" s="100" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="99"/>
-      <c r="B43" s="90"/>
-      <c r="C43" s="90"/>
-      <c r="D43" s="90"/>
-      <c r="E43" s="90"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="90"/>
-      <c r="H43" s="90"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="91"/>
-      <c r="K43" s="97" t="s">
+      <c r="A43" s="98"/>
+      <c r="B43" s="89"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="89"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
+      <c r="I43" s="90"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="L43" s="101" t="s">
+      <c r="L43" s="100" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="99"/>
-      <c r="B44" s="90"/>
-      <c r="C44" s="90"/>
-      <c r="D44" s="90"/>
-      <c r="E44" s="90"/>
-      <c r="F44" s="90"/>
-      <c r="G44" s="90"/>
-      <c r="H44" s="90"/>
-      <c r="I44" s="91"/>
-      <c r="J44" s="91"/>
-      <c r="K44" s="97" t="s">
+      <c r="A44" s="98"/>
+      <c r="B44" s="89"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="89"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="90"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="L44" s="101" t="s">
+      <c r="L44" s="100" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="99"/>
-      <c r="B45" s="90"/>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="90"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="97" t="s">
+      <c r="A45" s="98"/>
+      <c r="B45" s="89"/>
+      <c r="C45" s="89"/>
+      <c r="D45" s="89"/>
+      <c r="E45" s="89"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="90"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="L45" s="101" t="s">
+      <c r="L45" s="100" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="99"/>
-      <c r="B46" s="90"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="90"/>
-      <c r="H46" s="90"/>
-      <c r="I46" s="91"/>
-      <c r="J46" s="91"/>
-      <c r="K46" s="97" t="s">
+      <c r="A46" s="98"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="89"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="L46" s="101" t="s">
+      <c r="L46" s="100" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="99"/>
-      <c r="B47" s="90"/>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-      <c r="I47" s="91"/>
-      <c r="J47" s="91"/>
-      <c r="K47" s="97" t="s">
+      <c r="A47" s="98"/>
+      <c r="B47" s="89"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="89"/>
+      <c r="E47" s="89"/>
+      <c r="F47" s="89"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
+      <c r="I47" s="90"/>
+      <c r="J47" s="90"/>
+      <c r="K47" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="L47" s="101" t="s">
+      <c r="L47" s="100" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="99"/>
-      <c r="B48" s="90"/>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-      <c r="I48" s="91"/>
-      <c r="J48" s="91"/>
-      <c r="K48" s="97" t="s">
+      <c r="A48" s="98"/>
+      <c r="B48" s="89"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="89"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="89"/>
+      <c r="H48" s="89"/>
+      <c r="I48" s="90"/>
+      <c r="J48" s="90"/>
+      <c r="K48" s="96" t="s">
         <v>132</v>
       </c>
-      <c r="L48" s="101" t="s">
+      <c r="L48" s="100" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="99"/>
-      <c r="B49" s="90"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-      <c r="I49" s="91"/>
-      <c r="J49" s="91"/>
-      <c r="K49" s="97" t="s">
+      <c r="A49" s="98"/>
+      <c r="B49" s="89"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="89"/>
+      <c r="G49" s="89"/>
+      <c r="H49" s="89"/>
+      <c r="I49" s="90"/>
+      <c r="J49" s="90"/>
+      <c r="K49" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="L49" s="101" t="s">
+      <c r="L49" s="100" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="99"/>
-      <c r="B50" s="90"/>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="91"/>
-      <c r="J50" s="91"/>
-      <c r="K50" s="97" t="s">
+      <c r="A50" s="98"/>
+      <c r="B50" s="89"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
+      <c r="G50" s="89"/>
+      <c r="H50" s="89"/>
+      <c r="I50" s="90"/>
+      <c r="J50" s="90"/>
+      <c r="K50" s="96" t="s">
         <v>134</v>
       </c>
-      <c r="L50" s="101" t="s">
+      <c r="L50" s="100" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="99"/>
-      <c r="B51" s="90"/>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="90"/>
-      <c r="H51" s="90"/>
-      <c r="I51" s="91"/>
-      <c r="J51" s="91"/>
-      <c r="K51" s="97" t="s">
+      <c r="A51" s="98"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="89"/>
+      <c r="H51" s="89"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="96" t="s">
         <v>135</v>
       </c>
-      <c r="L51" s="101" t="s">
+      <c r="L51" s="100" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="99"/>
-      <c r="B52" s="90"/>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="90"/>
-      <c r="H52" s="90"/>
-      <c r="I52" s="91"/>
-      <c r="J52" s="91"/>
-      <c r="K52" s="97" t="s">
+      <c r="A52" s="98"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="89"/>
+      <c r="H52" s="89"/>
+      <c r="I52" s="90"/>
+      <c r="J52" s="90"/>
+      <c r="K52" s="96" t="s">
         <v>136</v>
       </c>
-      <c r="L52" s="101" t="s">
+      <c r="L52" s="100" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="99"/>
-      <c r="B53" s="90"/>
-      <c r="C53" s="90"/>
-      <c r="D53" s="90"/>
-      <c r="E53" s="90"/>
-      <c r="F53" s="90"/>
-      <c r="G53" s="90"/>
-      <c r="H53" s="90"/>
-      <c r="I53" s="91"/>
-      <c r="J53" s="91"/>
-      <c r="K53" s="97" t="s">
+      <c r="A53" s="98"/>
+      <c r="B53" s="89"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="89"/>
+      <c r="G53" s="89"/>
+      <c r="H53" s="89"/>
+      <c r="I53" s="90"/>
+      <c r="J53" s="90"/>
+      <c r="K53" s="96" t="s">
         <v>137</v>
       </c>
-      <c r="L53" s="95"/>
+      <c r="L53" s="94"/>
     </row>
     <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="99"/>
-      <c r="B54" s="90"/>
-      <c r="C54" s="90"/>
-      <c r="D54" s="90"/>
-      <c r="E54" s="90"/>
-      <c r="F54" s="90"/>
-      <c r="G54" s="90"/>
-      <c r="H54" s="90"/>
-      <c r="I54" s="91"/>
-      <c r="J54" s="91"/>
-      <c r="K54" s="103"/>
-      <c r="L54" s="95"/>
+      <c r="A54" s="98"/>
+      <c r="B54" s="89"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="89"/>
+      <c r="E54" s="89"/>
+      <c r="F54" s="89"/>
+      <c r="G54" s="89"/>
+      <c r="H54" s="89"/>
+      <c r="I54" s="90"/>
+      <c r="J54" s="90"/>
+      <c r="K54" s="102"/>
+      <c r="L54" s="94"/>
     </row>
     <row r="55" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="107"/>
-      <c r="B55" s="108"/>
-      <c r="C55" s="108"/>
-      <c r="D55" s="108"/>
-      <c r="E55" s="108"/>
-      <c r="F55" s="108"/>
-      <c r="G55" s="108"/>
-      <c r="H55" s="108"/>
-      <c r="I55" s="109"/>
-      <c r="J55" s="109"/>
-      <c r="K55" s="104"/>
-      <c r="L55" s="106"/>
+      <c r="A55" s="106"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="107"/>
+      <c r="D55" s="107"/>
+      <c r="E55" s="107"/>
+      <c r="F55" s="107"/>
+      <c r="G55" s="107"/>
+      <c r="H55" s="107"/>
+      <c r="I55" s="108"/>
+      <c r="J55" s="108"/>
+      <c r="K55" s="103"/>
+      <c r="L55" s="105"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>